<commit_message>
Update IP - EX 17 - Funcao arrumar (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 17 - Funcao arrumar (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 17 - Funcao arrumar (Anexo).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DD25CD8-9124-4096-BEBC-7FF8C1B8CD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581C386D-27AE-4994-84A7-71291DEA23CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>1. Função ARRUMAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Matheus Zambinati            </t>
-  </si>
-  <si>
     <t>Sem conteúdo nesta aula. ;)</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Função ARRUMAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matheus Zambinati                </t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -650,9 +650,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -698,12 +695,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
@@ -1507,96 +1500,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="38"/>
+      <c r="B2" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="40"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="44"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="43"/>
     </row>
     <row r="7" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,24 +1613,24 @@
       <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="34"/>
+      <c r="B9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="33"/>
     </row>
     <row r="10" spans="2:17" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -1685,7 +1678,7 @@
   <dimension ref="B2:Q87"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E10"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,97 +1693,97 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="str">
+      <c r="B2" s="35" t="str">
         <f>CONTEÚDO!B2</f>
         <v>Função ARRUMAR</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="38"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="41"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="40"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="41"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="40"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="43"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="43"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="44"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="43"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
@@ -1801,10 +1794,23 @@
     <row r="9" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="47" t="str">
+        <f>TRIM(B10)</f>
+        <v>Matheus Zambinati</v>
+      </c>
+      <c r="E10" s="48"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>LEN(B10)</f>
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <f>LEN(D10)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
@@ -1816,9 +1822,12 @@
       <c r="B15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="31"/>
+      <c r="C15" s="31" t="str">
+        <f>IF(B15="Lucas","Ok","Not Ok")</f>
+        <v>Ok</v>
+      </c>
       <c r="E15" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1826,32 +1835,37 @@
       <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="E17" s="32"/>
+      <c r="C17" s="31" t="str">
+        <f>IF(B17="Lucas","Ok","Not Ok")</f>
+        <v>Not Ok</v>
+      </c>
+      <c r="E17" s="31" t="str">
+        <f>IF(TRIM(B17)="Lucas","Ok","Not Ok")</f>
+        <v>Ok</v>
+      </c>
     </row>
     <row r="87" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C87" s="45" t="s">
+      <c r="C87" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="D87" s="46"/>
-      <c r="E87" s="46"/>
-      <c r="F87" s="46"/>
-      <c r="G87" s="46"/>
-      <c r="H87" s="46"/>
-      <c r="I87" s="46"/>
-      <c r="J87" s="46"/>
-      <c r="K87" s="46"/>
-      <c r="L87" s="46"/>
-      <c r="M87" s="46"/>
-      <c r="N87" s="46"/>
-      <c r="O87" s="46"/>
-      <c r="P87" s="47"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
+      <c r="G87" s="45"/>
+      <c r="H87" s="45"/>
+      <c r="I87" s="45"/>
+      <c r="J87" s="45"/>
+      <c r="K87" s="45"/>
+      <c r="L87" s="45"/>
+      <c r="M87" s="45"/>
+      <c r="N87" s="45"/>
+      <c r="O87" s="45"/>
+      <c r="P87" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="C87:P87"/>
     <mergeCell ref="B2:Q6"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1889,7 +1903,7 @@
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20"/>
       <c r="C4" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="22"/>
@@ -1904,7 +1918,7 @@
     </row>
     <row r="6" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
@@ -1921,7 +1935,7 @@
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20"/>
       <c r="C8" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
@@ -1937,7 +1951,7 @@
     <row r="10" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
       <c r="C10" s="27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
@@ -1953,7 +1967,7 @@
     <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20"/>
       <c r="C12" s="27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
@@ -1965,7 +1979,7 @@
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
       <c r="F13" s="30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>